<commit_message>
mejoras tras reunion, aditivo otra vez
</commit_message>
<xml_diff>
--- a/articulo 1 XAI/data_valencia_comunity/Resultados salida/3_data_complete_NN.xlsx
+++ b/articulo 1 XAI/data_valencia_comunity/Resultados salida/3_data_complete_NN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miumh-my.sharepoint.com/personal/ricardo_gonzalezm_miumh_umh_es/Documents/Documentos/Cafee/articulo 1 XAI/data_valencia_comunity/Resultados salida/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_A34693330069EDCB24E73CFA5F3D013B7259B285" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA3211BB-F120-4655-8813-C84C344EA619}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="11_A34693330069EDCB24E73CFA5F3D013B7259B285" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E71FF65-6736-449C-9C0E-9E5DD629D7EF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34680" yWindow="165" windowWidth="24660" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
   <si>
     <t>total_assets</t>
   </si>
@@ -103,22 +103,13 @@
     <t>0.98513</t>
   </si>
   <si>
-    <t>prob</t>
-  </si>
-  <si>
     <t>0.91</t>
   </si>
   <si>
     <t>0.95</t>
   </si>
   <si>
-    <t>0.96</t>
-  </si>
-  <si>
     <t>0.64</t>
-  </si>
-  <si>
-    <t>6.72</t>
   </si>
   <si>
     <t>0.2</t>
@@ -136,10 +127,22 @@
     <t>eff</t>
   </si>
   <si>
-    <t>efff</t>
+    <t>peer</t>
   </si>
   <si>
-    <t>peer</t>
+    <t>0.994</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.56</t>
+  </si>
+  <si>
+    <t>prob be eff</t>
   </si>
 </sst>
 </file>
@@ -269,7 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -574,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,10 +612,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I1" s="13"/>
       <c r="J1" t="s">
@@ -634,7 +637,7 @@
         <v>10</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="Q1" t="s">
         <v>11</v>
@@ -696,10 +699,10 @@
         <v>460.57785999999999</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2">
@@ -718,7 +721,7 @@
         <v>460.57785999999999</v>
       </c>
       <c r="O2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="P2">
         <v>1</v>
@@ -783,10 +786,10 @@
         <v>358.13</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J3">
         <v>184.97800000000001</v>
@@ -804,7 +807,7 @@
         <v>358.13</v>
       </c>
       <c r="O3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="P3">
         <v>2</v>
@@ -866,7 +869,7 @@
         <v>356.94675000000001</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -887,7 +890,7 @@
         <v>356.94675000000001</v>
       </c>
       <c r="O4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="P4">
         <v>3</v>
@@ -925,8 +928,8 @@
       <c r="AA4">
         <v>311.33477352452599</v>
       </c>
-      <c r="AB4">
-        <v>-0.79311853039801805</v>
+      <c r="AB4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
@@ -949,10 +952,10 @@
         <v>293.93365999999997</v>
       </c>
       <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
         <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
       </c>
       <c r="J5">
         <v>103.36555138664001</v>
@@ -1032,7 +1035,7 @@
         <v>268.27539999999999</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J6">
         <v>149.892303092551</v>
@@ -1111,6 +1114,9 @@
       <c r="F7">
         <v>259.06299999999999</v>
       </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
       <c r="J7">
         <v>156.47883410399899</v>
       </c>
@@ -1185,6 +1191,9 @@
       <c r="F8">
         <v>193.64809</v>
       </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
       <c r="J8">
         <v>116.36346033663401</v>
       </c>
@@ -1259,6 +1268,9 @@
       <c r="F9">
         <v>189.37</v>
       </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
       <c r="J9">
         <v>253.121296562775</v>
       </c>
@@ -1348,8 +1360,8 @@
       <c r="N10">
         <v>165.06169175550701</v>
       </c>
-      <c r="O10">
-        <v>-8.8934246974778294E-2</v>
+      <c r="O10" t="s">
+        <v>33</v>
       </c>
       <c r="Q10">
         <v>53.427918492939</v>
@@ -1366,8 +1378,8 @@
       <c r="U10">
         <v>169.69526134715301</v>
       </c>
-      <c r="V10">
-        <v>-8.3639628302428493E-3</v>
+      <c r="V10" t="s">
+        <v>33</v>
       </c>
       <c r="W10">
         <v>53.009975385113698</v>

</xml_diff>